<commit_message>
second code for auto-test
</commit_message>
<xml_diff>
--- a/tests/test_translate_plain_text_created_by_public_request/test_translate_plain_text_created_by_public_request.xlsx
+++ b/tests/test_translate_plain_text_created_by_public_request/test_translate_plain_text_created_by_public_request.xlsx
@@ -68,6 +68,17 @@
             <sz val="11"/>
             <rFont val="Calibri"/>
           </rPr>
+          <t xml:space="preserve">Clicks an Element</t>
+        </d:r>
+      </text>
+    </comment>
+    <comment ref="D32" authorId="0">
+      <text>
+        <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+          </rPr>
           <t xml:space="preserve">Wait for element to be visible &amp; have the defined text</t>
         </d:r>
       </text>
@@ -77,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t/>
   </si>
@@ -139,7 +150,7 @@
     <t>Last Modified on</t>
   </si>
   <si>
-    <t>04/03/2022 04:29:14</t>
+    <t>04/04/2022 01:17:57</t>
   </si>
   <si>
     <t>Web Application</t>
@@ -172,7 +183,7 @@
     <t>Input</t>
   </si>
   <si>
-    <t>Steps (5)</t>
+    <t>Steps (6)</t>
   </si>
   <si>
     <t>#</t>
@@ -265,13 +276,16 @@
     <t>keys=response</t>
   </si>
   <si>
-    <t>Click 'PHÁT HIỆN VÀ DỊCH' (Button)</t>
-  </si>
-  <si>
-    <t>Button: PHÁT HIỆN VÀ DỊCH (located by XPATH: //button[. = 'Phát hiện và dịch'])</t>
-  </si>
-  <si>
-    <t>5000ms After</t>
+    <t>Click 'ANH' (Button)</t>
+  </si>
+  <si>
+    <t>Button: ANH (located by XPATH: //button[. = 'Anh'])</t>
+  </si>
+  <si>
+    <t>Click 'DỊCH' (Button)</t>
+  </si>
+  <si>
+    <t>Button: DỊCH (located by XPATH: //button[. = 'Dịch'])</t>
   </si>
   <si>
     <t xml:space="preserve">Does 'phản ứng' (textarea) contain 'phản ứng xxx
@@ -473,7 +487,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TestParameters_Gy1ZU1o7" displayName="TestParameters_Gy1ZU1o7" ref="A22:D23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TestParameters_4gTz0QBd" displayName="TestParameters_4gTz0QBd" ref="A22:D23">
   <autoFilter ref="A22:D23"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Name"/>
@@ -486,8 +500,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Steps_fGAg0mXp" displayName="Steps_fGAg0mXp" ref="A26:O31">
-  <autoFilter ref="A26:O31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Steps_vv8ZAUvf" displayName="Steps_vv8ZAUvf" ref="A26:O32">
+  <autoFilter ref="A26:O32"/>
   <tableColumns count="15">
     <tableColumn id="1" name="#"/>
     <tableColumn id="2" name="Details"/>
@@ -511,7 +525,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -905,6 +919,9 @@
       <c r="B30" s="0" t="s">
         <v>62</v>
       </c>
+      <c r="C30" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="D30" s="0" t="s">
         <v>56</v>
       </c>
@@ -915,7 +932,7 @@
         <v>50</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="H30" s="0" t="s">
         <v>52</v>
@@ -943,49 +960,96 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="18">
+      <c r="A31" s="17">
         <v>5</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E31" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D31" s="12" t="s">
+      <c r="F31" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="I31" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="J31" s="0">
+        <v>1</v>
+      </c>
+      <c r="K31" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="L31" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M31" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="N31" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="O31" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="18">
+        <v>6</v>
+      </c>
+      <c r="B32" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="C32" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="F31" s="12" t="s">
+      <c r="E32" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F32" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="G31" s="12" t="s">
+      <c r="G32" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="H31" s="12" t="s">
+      <c r="H32" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="I31" s="12" t="s">
+      <c r="I32" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="J31" s="12">
+      <c r="J32" s="12">
         <v>1</v>
       </c>
-      <c r="K31" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="L31" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="M31" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="N31" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="O31" s="16" t="b">
+      <c r="K32" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="L32" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="M32" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N32" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="O32" s="16" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>